<commit_message>
finalizei cobertura e curva abc da bibi
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/metricas_analise_estoque.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/metricas_analise_estoque.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>DATA_HORA_ANALISE</t>
   </si>
@@ -25,25 +25,25 @@
     <t>TOTAL SKU COM VENDA ACIMA DE 1 ANO</t>
   </si>
   <si>
-    <t>% SKU COM VENDA ACIMA DE 1 ANO</t>
-  </si>
-  <si>
-    <t>TOTAL SKU COM VENDA SOMENTE NO ÚLTIMO ANO</t>
-  </si>
-  <si>
-    <t>% SKU COM VENDA SOMENTE NO ÚLTIMO ANO</t>
+    <t>%SKU COM VENDA ACIMA DE 1 ANO</t>
+  </si>
+  <si>
+    <t>TOTAL SKU COM VENDA SOMENTE NO ULTIMO ANO</t>
+  </si>
+  <si>
+    <t>%SKU COM VENDA SOMENTE NO ULTIMO ANO</t>
   </si>
   <si>
     <t>TOTAL SKU COM ESTOQUE ZERO</t>
   </si>
   <si>
-    <t>% SKU COM ESTOQUE ZERO</t>
+    <t>%SKU COM ESTOQUE ZERO</t>
   </si>
   <si>
     <t>TOTAL SKU COM ESTOQUE POSITIVO</t>
   </si>
   <si>
-    <t>% SKU COM ESTOQUE POSITIVO</t>
+    <t>%SKU COM ESTOQUE POSITIVO</t>
   </si>
   <si>
     <t>CUSTO TOTAL ESTOQUE POSITIVO</t>
@@ -52,55 +52,55 @@
     <t>TOTAL SKU COM ESTOQUE NEGATIVO</t>
   </si>
   <si>
-    <t>% SKU COM ESTOQUE NEGATIVO</t>
+    <t>%SKU COM ESTOQUE NEGATIVO</t>
   </si>
   <si>
     <t>CUSTO TOTAL ESTOQUE NEGATIVO</t>
   </si>
   <si>
-    <t>TOTAL SKU inativo com Saldo</t>
-  </si>
-  <si>
-    <t>% SKU INATIVO COM SALDO</t>
+    <t>TOTAL SKU INATIVO COM SALDO</t>
+  </si>
+  <si>
+    <t>%SKU INATIVO COM SALDO</t>
   </si>
   <si>
     <t>CUSTO TOTAL INATIVO COM SALDO</t>
   </si>
   <si>
-    <t>TOTAL SKU Inativo sem Saldo</t>
-  </si>
-  <si>
-    <t>% SKU INATIVO SEM SALDO</t>
-  </si>
-  <si>
-    <t>TOTAL SKU Ativo com Saldo</t>
-  </si>
-  <si>
-    <t>% SKU ATIVO COM SALDO</t>
+    <t>TOTAL SKU INATIVO SEM SALDO</t>
+  </si>
+  <si>
+    <t>%SKU INATIVO SEM SALDO</t>
+  </si>
+  <si>
+    <t>TOTAL SKU ATIVO COM SALDO</t>
+  </si>
+  <si>
+    <t>%SKU ATIVO COM SALDO</t>
   </si>
   <si>
     <t>CUSTO TOTAL ATIVO COM SALDO</t>
   </si>
   <si>
-    <t>TOTAL SKU Ativo sem Saldo</t>
-  </si>
-  <si>
-    <t>% SKU ATIVO SEM SALDO</t>
-  </si>
-  <si>
-    <t>TOTAL SKU SEM VENDA com Saldo</t>
-  </si>
-  <si>
-    <t>% SKU SEM VENDA COM SALDO</t>
+    <t>TOTAL SKU ATIVO SEM SALDO</t>
+  </si>
+  <si>
+    <t>%SKU ATIVO SEM SALDO</t>
+  </si>
+  <si>
+    <t>TOTAL SKU SEM VENDA COM SALDO</t>
+  </si>
+  <si>
+    <t>%SKU SEM VENDA COM SALDO</t>
   </si>
   <si>
     <t>CUSTO TOTAL SEM VENDA COM SALDO</t>
   </si>
   <si>
-    <t>TOTAL SKU SEM VENDA sem Saldo</t>
-  </si>
-  <si>
-    <t>% SKU SEM VENDA SEM SALDO</t>
+    <t>TOTAL SKU SEM VENDA SEM SALDO</t>
+  </si>
+  <si>
+    <t>%SKU SEM VENDA SEM SALDO</t>
   </si>
   <si>
     <t>TOTAL SKU GRUPO A</t>
@@ -112,13 +112,13 @@
     <t>TOTAL SKU GRUPO C</t>
   </si>
   <si>
-    <t>% SKU GRUPO A</t>
+    <t>%SKU GRUPO A</t>
   </si>
   <si>
     <t>%SKU GRUPO B</t>
   </si>
   <si>
-    <t>% SKU GRUPO C</t>
+    <t>%SKU GRUPO C</t>
   </si>
   <si>
     <t>TOTAL VENDA GRUPO A</t>
@@ -130,16 +130,13 @@
     <t>TOTAL VENDA GRUPO C</t>
   </si>
   <si>
-    <t>% VENDA GRUPO A</t>
-  </si>
-  <si>
-    <t>% VENDA GRUPO B</t>
-  </si>
-  <si>
-    <t>% VENDA GRUPO C</t>
-  </si>
-  <si>
-    <t>COBERTURA EM DIAS</t>
+    <t>%VENDA GRUPO A</t>
+  </si>
+  <si>
+    <t>%VENDA GRUPO B</t>
+  </si>
+  <si>
+    <t>%VENDA GRUPO C</t>
   </si>
   <si>
     <t>COBERTURA EM DIAS GRUPO A</t>
@@ -151,7 +148,7 @@
     <t>COBERTURA EM DIAS GRUPO C</t>
   </si>
   <si>
-    <t>2025-05-08 15:47:00</t>
+    <t>2025-05-09 18:54:59</t>
   </si>
 </sst>
 </file>
@@ -509,13 +506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS2"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:45">
+    <row r="1" spans="1:44">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,145 +645,139 @@
       <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:44">
+      <c r="A2" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:45">
-      <c r="A2" t="s">
-        <v>45</v>
-      </c>
       <c r="B2">
-        <v>1004</v>
+        <v>16142</v>
       </c>
       <c r="C2">
-        <v>447</v>
+        <v>11643</v>
       </c>
       <c r="D2">
-        <v>44.52191235059761</v>
+        <v>72.12860859868667</v>
       </c>
       <c r="E2">
-        <v>535</v>
+        <v>2277</v>
       </c>
       <c r="F2">
-        <v>53.28685258964143</v>
+        <v>14.10605872878206</v>
       </c>
       <c r="G2">
-        <v>90</v>
+        <v>3094</v>
       </c>
       <c r="H2">
-        <v>8.964143426294822</v>
+        <v>19.1673894189072</v>
       </c>
       <c r="I2">
-        <v>640</v>
+        <v>9526</v>
       </c>
       <c r="J2">
-        <v>63.74501992031873</v>
+        <v>59.01375294263412</v>
       </c>
       <c r="K2">
-        <v>14134</v>
+        <v>3036032.85</v>
       </c>
       <c r="L2">
-        <v>274</v>
+        <v>3522</v>
       </c>
       <c r="M2">
-        <v>27.29083665338645</v>
+        <v>21.81885763845868</v>
       </c>
       <c r="N2">
-        <v>5622</v>
+        <v>1072804.73</v>
       </c>
       <c r="O2">
-        <v>3</v>
+        <v>4623</v>
       </c>
       <c r="P2">
-        <v>0.298804780876494</v>
+        <v>28.63957378267873</v>
       </c>
       <c r="Q2">
-        <v>40</v>
+        <v>473467.8999999999</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>3502</v>
       </c>
       <c r="S2">
-        <v>0.099601593625498</v>
+        <v>21.69495725436749</v>
       </c>
       <c r="T2">
-        <v>619</v>
+        <v>3484</v>
       </c>
       <c r="U2">
-        <v>61.65338645418327</v>
+        <v>21.58344690868542</v>
       </c>
       <c r="V2">
-        <v>13970</v>
+        <v>2422321.85</v>
       </c>
       <c r="W2">
-        <v>359</v>
+        <v>2311</v>
       </c>
       <c r="X2">
-        <v>35.75697211155379</v>
+        <v>14.31668938173708</v>
       </c>
       <c r="Y2">
-        <v>18</v>
+        <v>1419</v>
       </c>
       <c r="Z2">
-        <v>1.792828685258964</v>
+        <v>8.790732251269979</v>
       </c>
       <c r="AA2">
-        <v>124</v>
+        <v>140243.1</v>
       </c>
       <c r="AB2">
-        <v>4</v>
+        <v>803</v>
       </c>
       <c r="AC2">
-        <v>0.398406374501992</v>
+        <v>4.974600421261306</v>
       </c>
       <c r="AD2">
-        <v>238</v>
+        <v>463</v>
       </c>
       <c r="AE2">
-        <v>294</v>
+        <v>878</v>
       </c>
       <c r="AF2">
-        <v>426</v>
+        <v>1389</v>
       </c>
       <c r="AG2">
-        <v>23.70517928286853</v>
+        <v>16.95970695970696</v>
       </c>
       <c r="AH2">
-        <v>29.28286852589641</v>
+        <v>32.16117216117216</v>
       </c>
       <c r="AI2">
-        <v>42.43027888446215</v>
+        <v>50.87912087912088</v>
       </c>
       <c r="AJ2">
-        <v>731895.1399999999</v>
+        <v>1422342.64</v>
       </c>
       <c r="AK2">
-        <v>137239.85</v>
+        <v>266803.27</v>
       </c>
       <c r="AL2">
-        <v>45864.07</v>
+        <v>89026.19</v>
       </c>
       <c r="AM2">
-        <v>79.98862206481392</v>
+        <v>79.98903143289674</v>
       </c>
       <c r="AN2">
-        <v>14.99890611909482</v>
+        <v>15.00435587758913</v>
       </c>
       <c r="AO2">
-        <v>5.012471816091265</v>
+        <v>5.006612689514137</v>
       </c>
       <c r="AP2">
-        <v>376.4790414264245</v>
+        <v>47.69122524876872</v>
       </c>
       <c r="AQ2">
-        <v>99.94312760960767</v>
+        <v>224.0439682246444</v>
       </c>
       <c r="AR2">
-        <v>163.5770236308493</v>
-      </c>
-      <c r="AS2">
-        <v>707.4191019122585</v>
+        <v>568.357470858354</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tentativa de colocar os dados de curva e cobertura no dash
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/metricas_analise_estoque.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/metricas_analise_estoque.xlsx
@@ -22,16 +22,16 @@
     <t>TOTAL DE SKUs</t>
   </si>
   <si>
-    <t>TOTAL SKU COM VENDA ACIMA DE 1 ANO</t>
-  </si>
-  <si>
-    <t>%SKU COM VENDA ACIMA DE 1 ANO</t>
-  </si>
-  <si>
-    <t>TOTAL SKU COM VENDA SOMENTE NO ULTIMO ANO</t>
-  </si>
-  <si>
-    <t>%SKU COM VENDA SOMENTE NO ULTIMO ANO</t>
+    <t>TOTAL SKU COM HISTORICO &gt; 1 ANO</t>
+  </si>
+  <si>
+    <t>%SKU COM COM HISTORICO &gt; 1 ANO</t>
+  </si>
+  <si>
+    <t>TOTAL SKU COM HISTORICO &lt; 1 ANO</t>
+  </si>
+  <si>
+    <t>%SKU COM HISTORICO &lt; 1 ANO</t>
   </si>
   <si>
     <t>TOTAL SKU COM ESTOQUE ZERO</t>
@@ -58,64 +58,64 @@
     <t>CUSTO TOTAL ESTOQUE NEGATIVO</t>
   </si>
   <si>
-    <t>TOTAL SKU INATIVO COM SALDO</t>
-  </si>
-  <si>
-    <t>%SKU INATIVO COM SALDO</t>
-  </si>
-  <si>
-    <t>CUSTO TOTAL INATIVO COM SALDO</t>
-  </si>
-  <si>
-    <t>TOTAL SKU INATIVO SEM SALDO</t>
-  </si>
-  <si>
-    <t>%SKU INATIVO SEM SALDO</t>
-  </si>
-  <si>
-    <t>TOTAL SKU ATIVO COM SALDO</t>
-  </si>
-  <si>
-    <t>%SKU ATIVO COM SALDO</t>
-  </si>
-  <si>
-    <t>CUSTO TOTAL ATIVO COM SALDO</t>
-  </si>
-  <si>
-    <t>TOTAL SKU ATIVO SEM SALDO</t>
-  </si>
-  <si>
-    <t>%SKU ATIVO SEM SALDO</t>
-  </si>
-  <si>
-    <t>TOTAL SKU SEM VENDA COM SALDO</t>
-  </si>
-  <si>
-    <t>%SKU SEM VENDA COM SALDO</t>
-  </si>
-  <si>
-    <t>CUSTO TOTAL SEM VENDA COM SALDO</t>
-  </si>
-  <si>
-    <t>TOTAL SKU SEM VENDA SEM SALDO</t>
-  </si>
-  <si>
-    <t>%SKU SEM VENDA SEM SALDO</t>
-  </si>
-  <si>
-    <t>TOTAL SKUs VERIFICADOS</t>
-  </si>
-  <si>
-    <t>TOTAL SKUs CONSISTENTES</t>
-  </si>
-  <si>
-    <t>%SKUs CONSISTENTES</t>
-  </si>
-  <si>
-    <t>TOTAL SKUs INCONSISTENTES</t>
-  </si>
-  <si>
-    <t>%SKUs INCONSISTENTES</t>
+    <t>TOTAL SKU INATIVO (ESTOQUE &gt; 0)</t>
+  </si>
+  <si>
+    <t>%SKU INATIVO (ESTOQUE &gt; 0)</t>
+  </si>
+  <si>
+    <t>CUSTO TOTAL INATIVO (ESTOQUE &gt; 0)</t>
+  </si>
+  <si>
+    <t>TOTAL SKU INATIVO (ESTOQUE &lt;= 0)</t>
+  </si>
+  <si>
+    <t>%SKU INATIVO (ESTOQUE &lt;= 0)</t>
+  </si>
+  <si>
+    <t>TOTAL SKU ATIVO (ESTOQUE &gt; 0)</t>
+  </si>
+  <si>
+    <t>%SKU ATIVO (ESTOQUE &gt; 0)</t>
+  </si>
+  <si>
+    <t>CUSTO TOTAL ATIVO (ESTOQUE &gt; 0)</t>
+  </si>
+  <si>
+    <t>TOTAL SKU ATIVO (ESTOQUE &lt;= 0)</t>
+  </si>
+  <si>
+    <t>%SKU ATIVO (ESTOQUE &lt;= 0)</t>
+  </si>
+  <si>
+    <t>TOTAL SKU NAO COMERCIALIZADO (ESTOQUE &gt; 0)</t>
+  </si>
+  <si>
+    <t>%SKU NAO COMERCIALIZADO (ESTOQUE &gt; 0)</t>
+  </si>
+  <si>
+    <t>CUSTO TOTAL NAO COMERCIALIZADO (ESTOQUE &gt; 0)</t>
+  </si>
+  <si>
+    <t>TOTAL SKU NAO COMERCIALIZADO (ESTOQUE &lt;= 0)</t>
+  </si>
+  <si>
+    <t>%SKU NAO COMERCIALIZADO (ESTOQUE &lt;= 0)</t>
+  </si>
+  <si>
+    <t>TOTAL SKU VERIFICADOS</t>
+  </si>
+  <si>
+    <t>TOTAL SKU CONSISTENTES</t>
+  </si>
+  <si>
+    <t>%SKU CONSISTENTES</t>
+  </si>
+  <si>
+    <t>TOTAL SKU INCONSISTENTES</t>
+  </si>
+  <si>
+    <t>%SKU INCONSISTENTES</t>
   </si>
   <si>
     <t>TOTAL SKU GRUPO A</t>
@@ -163,7 +163,7 @@
     <t>COBERTURA EM DIAS GRUPO C</t>
   </si>
   <si>
-    <t>2025-05-14 11:03:59</t>
+    <t>2025-05-14 14:32:31</t>
   </si>
 </sst>
 </file>
@@ -684,16 +684,16 @@
         <v>16151</v>
       </c>
       <c r="C2">
-        <v>11663</v>
+        <v>11664</v>
       </c>
       <c r="D2">
-        <v>72.21224691969537</v>
+        <v>72.218438486781</v>
       </c>
       <c r="E2">
-        <v>2278</v>
+        <v>2277</v>
       </c>
       <c r="F2">
-        <v>14.10438982106371</v>
+        <v>14.09819825397808</v>
       </c>
       <c r="G2">
         <v>3099</v>
@@ -729,10 +729,10 @@
         <v>482277.6</v>
       </c>
       <c r="R2">
-        <v>3519</v>
+        <v>3520</v>
       </c>
       <c r="S2">
-        <v>21.78812457432976</v>
+        <v>21.79431614141539</v>
       </c>
       <c r="T2">
         <v>3468</v>
@@ -744,10 +744,10 @@
         <v>2425841.56</v>
       </c>
       <c r="W2">
-        <v>2306</v>
+        <v>2305</v>
       </c>
       <c r="X2">
-        <v>14.27775369946133</v>
+        <v>14.2715621323757</v>
       </c>
       <c r="Y2">
         <v>1408</v>
@@ -780,49 +780,49 @@
         <v>34.4861721215121</v>
       </c>
       <c r="AI2">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="AJ2">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="AK2">
-        <v>1392</v>
+        <v>1390</v>
       </c>
       <c r="AL2">
-        <v>16.8076498712762</v>
+        <v>16.79558011049724</v>
       </c>
       <c r="AM2">
-        <v>31.99705774181684</v>
+        <v>32.00736648250461</v>
       </c>
       <c r="AN2">
-        <v>51.19529238690696</v>
+        <v>51.19705340699816</v>
       </c>
       <c r="AO2">
-        <v>1424447.37</v>
+        <v>1421923.25</v>
       </c>
       <c r="AP2">
-        <v>267435.48</v>
+        <v>266876.46</v>
       </c>
       <c r="AQ2">
-        <v>89098.85000000001</v>
+        <v>88904.47</v>
       </c>
       <c r="AR2">
-        <v>79.9810222642939</v>
+        <v>79.98649415337484</v>
       </c>
       <c r="AS2">
-        <v>15.0161834902627</v>
+        <v>15.01242237052061</v>
       </c>
       <c r="AT2">
-        <v>5.002794245443398</v>
+        <v>5.001083476104556</v>
       </c>
       <c r="AU2">
-        <v>44.60963206700568</v>
+        <v>44.79682953747366</v>
       </c>
       <c r="AV2">
-        <v>210.5537459283388</v>
+        <v>207.5719717544813</v>
       </c>
       <c r="AW2">
-        <v>563.4796348314607</v>
+        <v>567.1548998946259</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finalizei estoque bibi no dash
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/metricas_analise_estoque.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/metricas_analise_estoque.xlsx
@@ -163,7 +163,7 @@
     <t>COBERTURA EM DIAS GRUPO C</t>
   </si>
   <si>
-    <t>2025-05-14 14:32:31</t>
+    <t>2025-05-22 15:29:05</t>
   </si>
 </sst>
 </file>
@@ -681,148 +681,148 @@
         <v>49</v>
       </c>
       <c r="B2">
-        <v>16151</v>
+        <v>16217</v>
       </c>
       <c r="C2">
-        <v>11664</v>
+        <v>11724</v>
       </c>
       <c r="D2">
-        <v>72.218438486781</v>
+        <v>72.29450576555466</v>
       </c>
       <c r="E2">
-        <v>2277</v>
+        <v>2247</v>
       </c>
       <c r="F2">
-        <v>14.09819825397808</v>
+        <v>13.85583030153543</v>
       </c>
       <c r="G2">
-        <v>3099</v>
+        <v>3106</v>
       </c>
       <c r="H2">
-        <v>19.18766639836543</v>
+        <v>19.15274095085404</v>
       </c>
       <c r="I2">
-        <v>9524</v>
+        <v>9561</v>
       </c>
       <c r="J2">
-        <v>58.96848492353415</v>
+        <v>58.95665042856262</v>
       </c>
       <c r="K2">
-        <v>3042558.26</v>
+        <v>3080559.16</v>
       </c>
       <c r="L2">
-        <v>3528</v>
+        <v>3550</v>
       </c>
       <c r="M2">
-        <v>21.84384867810043</v>
+        <v>21.89060862058334</v>
       </c>
       <c r="N2">
-        <v>1101515.63</v>
+        <v>1136656.43</v>
       </c>
       <c r="O2">
-        <v>4648</v>
+        <v>4672</v>
       </c>
       <c r="P2">
-        <v>28.77840381400533</v>
+        <v>28.80927421841278</v>
       </c>
       <c r="Q2">
-        <v>482277.6</v>
+        <v>489961.1</v>
       </c>
       <c r="R2">
-        <v>3520</v>
+        <v>3544</v>
       </c>
       <c r="S2">
-        <v>21.79431614141539</v>
+        <v>21.85361040883024</v>
       </c>
       <c r="T2">
-        <v>3468</v>
+        <v>3449</v>
       </c>
       <c r="U2">
-        <v>21.47235465296266</v>
+        <v>21.26780538940618</v>
       </c>
       <c r="V2">
-        <v>2425841.56</v>
+        <v>2436238.06</v>
       </c>
       <c r="W2">
-        <v>2305</v>
+        <v>2306</v>
       </c>
       <c r="X2">
-        <v>14.2715621323757</v>
+        <v>14.2196460504409</v>
       </c>
       <c r="Y2">
-        <v>1408</v>
+        <v>1440</v>
       </c>
       <c r="Z2">
-        <v>8.717726456566156</v>
+        <v>8.879570820743664</v>
       </c>
       <c r="AA2">
-        <v>134439.1</v>
+        <v>154360</v>
       </c>
       <c r="AB2">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="AC2">
-        <v>4.965636802674757</v>
+        <v>4.970093112166245</v>
       </c>
       <c r="AD2">
-        <v>16163</v>
+        <v>16229</v>
       </c>
       <c r="AE2">
-        <v>10589</v>
+        <v>10598</v>
       </c>
       <c r="AF2">
-        <v>65.5138278784879</v>
+        <v>65.30285291761662</v>
       </c>
       <c r="AG2">
-        <v>5574</v>
+        <v>5631</v>
       </c>
       <c r="AH2">
-        <v>34.4861721215121</v>
+        <v>34.69714708238338</v>
       </c>
       <c r="AI2">
-        <v>456</v>
+        <v>466</v>
       </c>
       <c r="AJ2">
-        <v>869</v>
+        <v>864</v>
       </c>
       <c r="AK2">
-        <v>1390</v>
+        <v>1366</v>
       </c>
       <c r="AL2">
-        <v>16.79558011049724</v>
+        <v>17.28486646884273</v>
       </c>
       <c r="AM2">
-        <v>32.00736648250461</v>
+        <v>32.04747774480713</v>
       </c>
       <c r="AN2">
-        <v>51.19705340699816</v>
+        <v>50.66765578635015</v>
       </c>
       <c r="AO2">
-        <v>1421923.25</v>
+        <v>1381340.64</v>
       </c>
       <c r="AP2">
-        <v>266876.46</v>
+        <v>259487.28</v>
       </c>
       <c r="AQ2">
-        <v>88904.47</v>
+        <v>86475.97</v>
       </c>
       <c r="AR2">
-        <v>79.98649415337484</v>
+        <v>79.97091004061826</v>
       </c>
       <c r="AS2">
-        <v>15.01242237052061</v>
+        <v>15.02267675666498</v>
       </c>
       <c r="AT2">
-        <v>5.001083476104556</v>
+        <v>5.006413202716749</v>
       </c>
       <c r="AU2">
-        <v>44.79682953747366</v>
+        <v>46.24280782508631</v>
       </c>
       <c r="AV2">
-        <v>207.5719717544813</v>
+        <v>233.1918505942275</v>
       </c>
       <c r="AW2">
-        <v>567.1548998946259</v>
+        <v>558.110151187905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
atualizei os dados da bibi
</commit_message>
<xml_diff>
--- a/dados/BIBI/Dados_BIBI_PF/metricas_analise_estoque.xlsx
+++ b/dados/BIBI/Dados_BIBI_PF/metricas_analise_estoque.xlsx
@@ -163,7 +163,7 @@
     <t>COBERTURA EM DIAS GRUPO C</t>
   </si>
   <si>
-    <t>2025-05-25 18:32:19</t>
+    <t>2025-05-26 17:28:57</t>
   </si>
 </sst>
 </file>
@@ -684,16 +684,16 @@
         <v>16229</v>
       </c>
       <c r="C2">
-        <v>11751</v>
+        <v>11756</v>
       </c>
       <c r="D2">
-        <v>72.40741881816501</v>
+        <v>72.43822786370077</v>
       </c>
       <c r="E2">
-        <v>2241</v>
+        <v>2236</v>
       </c>
       <c r="F2">
-        <v>13.8086142091318</v>
+        <v>13.77780516359603</v>
       </c>
       <c r="G2">
         <v>3105</v>
@@ -720,34 +720,34 @@
         <v>1158493.43</v>
       </c>
       <c r="O2">
-        <v>4689</v>
+        <v>4695</v>
       </c>
       <c r="P2">
-        <v>28.89272290344445</v>
+        <v>28.92969375808738</v>
       </c>
       <c r="Q2">
-        <v>494295.3</v>
+        <v>497862.3</v>
       </c>
       <c r="R2">
-        <v>3569</v>
+        <v>3572</v>
       </c>
       <c r="S2">
-        <v>21.99149670343213</v>
+        <v>22.00998213075359</v>
       </c>
       <c r="T2">
-        <v>3435</v>
+        <v>3429</v>
       </c>
       <c r="U2">
-        <v>21.16581428307351</v>
+        <v>21.12884342843059</v>
       </c>
       <c r="V2">
-        <v>2427830.57</v>
+        <v>2424263.57</v>
       </c>
       <c r="W2">
-        <v>2299</v>
+        <v>2296</v>
       </c>
       <c r="X2">
-        <v>14.16599913734672</v>
+        <v>14.14751371002526</v>
       </c>
       <c r="Y2">
         <v>1434</v>
@@ -780,49 +780,49 @@
         <v>34.66535311865033</v>
       </c>
       <c r="AI2">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="AJ2">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="AK2">
-        <v>1354</v>
+        <v>1339</v>
       </c>
       <c r="AL2">
-        <v>17.74731381993331</v>
+        <v>18.01935964259122</v>
       </c>
       <c r="AM2">
-        <v>32.08595776213413</v>
+        <v>32.12956068503351</v>
       </c>
       <c r="AN2">
-        <v>50.16672841793257</v>
+        <v>49.85107967237528</v>
       </c>
       <c r="AO2">
-        <v>1360191</v>
+        <v>1331527.2</v>
       </c>
       <c r="AP2">
-        <v>255433.51</v>
+        <v>249630.26</v>
       </c>
       <c r="AQ2">
-        <v>85168.91</v>
+        <v>83316.29000000001</v>
       </c>
       <c r="AR2">
-        <v>79.97391005898884</v>
+        <v>79.99688790526135</v>
       </c>
       <c r="AS2">
-        <v>15.01849119336316</v>
+        <v>14.99754862460282</v>
       </c>
       <c r="AT2">
-        <v>5.007598747648025</v>
+        <v>5.005563470135831</v>
       </c>
       <c r="AU2">
-        <v>49.75165717486696</v>
+        <v>50.29909706546275</v>
       </c>
       <c r="AV2">
-        <v>239.0586868099942</v>
+        <v>234.8590021691974</v>
       </c>
       <c r="AW2">
-        <v>535.3431192660551</v>
+        <v>552.6344878408254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>